<commit_message>
data may be ok
</commit_message>
<xml_diff>
--- a/statistics/general.xlsx
+++ b/statistics/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\ForumPolarization\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D7C804-9F13-40D8-915F-D4A6FCFCDEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C72F42-059F-4C79-B341-DB508D45E3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +103,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -124,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -135,9 +150,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,7 +439,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,18 +454,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -481,91 +499,91 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>104927</v>
+        <v>143116</v>
       </c>
       <c r="C3">
-        <v>80</v>
+        <v>222</v>
       </c>
       <c r="D3">
-        <v>2203</v>
+        <v>3395</v>
       </c>
       <c r="E3">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="F3">
-        <v>102125</v>
+        <v>146511</v>
       </c>
       <c r="G3">
-        <v>148</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>9850</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="6">
+        <v>118139</v>
+      </c>
+      <c r="C4" s="6">
+        <v>216</v>
+      </c>
+      <c r="D4" s="6">
+        <v>14939</v>
+      </c>
+      <c r="E4" s="6">
+        <v>58</v>
+      </c>
+      <c r="F4" s="6">
+        <v>132278</v>
+      </c>
+      <c r="G4" s="6">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4">
-        <v>5271</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>15121</v>
-      </c>
-      <c r="G4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
+      <c r="B5" s="7">
         <v>5329</v>
       </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="7">
+        <v>139</v>
+      </c>
+      <c r="D5" s="7">
         <v>175</v>
       </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="7">
+        <v>15</v>
+      </c>
+      <c r="F5" s="7">
         <v>5504</v>
       </c>
-      <c r="G5">
-        <v>20</v>
+      <c r="G5" s="7">
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>9451</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>1599</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>11050</v>
-      </c>
-      <c r="G6">
-        <v>18</v>
+      <c r="B6" s="6">
+        <v>68068</v>
+      </c>
+      <c r="C6" s="6">
+        <v>139</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1897</v>
+      </c>
+      <c r="E6" s="6">
+        <v>15</v>
+      </c>
+      <c r="F6" s="6">
+        <v>69965</v>
+      </c>
+      <c r="G6" s="6">
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -573,37 +591,37 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>2101</v>
-      </c>
-      <c r="C7">
+        <v>41082</v>
+      </c>
+      <c r="C7" s="6">
+        <v>221</v>
+      </c>
+      <c r="D7" s="6">
+        <v>24904</v>
+      </c>
+      <c r="E7" s="6">
+        <v>576</v>
+      </c>
+      <c r="F7" s="6">
+        <v>65656</v>
+      </c>
+      <c r="G7" s="6">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D7">
-        <v>1244</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>3345</v>
-      </c>
-      <c r="G7">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -633,22 +651,22 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>62232</v>
+        <v>58497</v>
       </c>
       <c r="C11">
-        <v>91145</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1363</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1742</v>
-      </c>
-      <c r="F11" s="5">
-        <v>62232</v>
-      </c>
-      <c r="G11" s="5">
-        <v>91145</v>
+        <v>88738</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1361</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1711</v>
+      </c>
+      <c r="F11" s="6">
+        <v>59133</v>
+      </c>
+      <c r="G11" s="6">
+        <v>89884</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -744,18 +762,18 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="8"/>
+      <c r="D20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="8"/>
+      <c r="F20" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="6"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">

</xml_diff>

<commit_message>
FINAL COMMIT BEFORE UPDATE
</commit_message>
<xml_diff>
--- a/statistics/general.xlsx
+++ b/statistics/general.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\ForumPolarization\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB4F7D1-C545-4043-9928-24E67E6BF038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807D7AC7-B875-480C-89E4-73449314CAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -417,49 +417,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,24 +759,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43" t="s">
+      <c r="C1" s="53"/>
+      <c r="D1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="53"/>
+      <c r="F1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="52"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
+      <c r="A2" s="51"/>
       <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
@@ -796,21 +795,21 @@
       <c r="G2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="51"/>
-      <c r="M2" s="44" t="s">
+      <c r="L2" s="45"/>
+      <c r="M2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44" t="s">
+      <c r="N2" s="46"/>
+      <c r="O2" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="45"/>
+      <c r="P2" s="47"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -834,7 +833,7 @@
       <c r="G3" s="17">
         <v>339</v>
       </c>
-      <c r="J3" s="49"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="33" t="s">
         <v>5</v>
       </c>
@@ -1048,21 +1047,21 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J9" s="48" t="s">
+      <c r="J9" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="51" t="s">
+      <c r="K9" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="51"/>
-      <c r="M9" s="44" t="s">
+      <c r="L9" s="45"/>
+      <c r="M9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44" t="s">
+      <c r="N9" s="46"/>
+      <c r="O9" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="P9" s="45"/>
+      <c r="P9" s="47"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
@@ -1072,7 +1071,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="J10" s="49"/>
+      <c r="J10" s="44"/>
       <c r="K10" s="38" t="s">
         <v>5</v>
       </c>
@@ -1119,17 +1118,17 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43" t="s">
+      <c r="C12" s="53"/>
+      <c r="D12" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="43"/>
+      <c r="E12" s="53"/>
       <c r="F12" s="14" t="s">
         <v>9</v>
       </c>
@@ -1148,7 +1147,7 @@
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="26" t="s">
         <v>5</v>
       </c>
@@ -1565,7 +1564,7 @@
       <c r="L27">
         <v>2</v>
       </c>
-      <c r="M27" s="54">
+      <c r="M27" s="1">
         <v>48</v>
       </c>
     </row>
@@ -1587,17 +1586,17 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43" t="s">
+      <c r="C29" s="53"/>
+      <c r="D29" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="43"/>
+      <c r="E29" s="53"/>
       <c r="F29" s="14" t="s">
         <v>9</v>
       </c>
@@ -1616,7 +1615,7 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="26" t="s">
         <v>5</v>
       </c>
@@ -1667,7 +1666,7 @@
       <c r="F31" s="10">
         <v>82554</v>
       </c>
-      <c r="G31" s="53">
+      <c r="G31" s="40">
         <v>152780</v>
       </c>
       <c r="J31" s="23" t="s">
@@ -1739,10 +1738,10 @@
       <c r="C34" s="2">
         <v>93995</v>
       </c>
-      <c r="D34" s="55">
+      <c r="D34" s="41">
         <v>53</v>
       </c>
-      <c r="E34" s="55">
+      <c r="E34" s="41">
         <v>61</v>
       </c>
       <c r="F34" s="2">
@@ -1779,22 +1778,22 @@
       <c r="A36" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="55">
+      <c r="B36" s="41">
         <v>15621</v>
       </c>
-      <c r="C36" s="55">
+      <c r="C36" s="41">
         <v>31267</v>
       </c>
-      <c r="D36" s="55">
+      <c r="D36" s="41">
         <v>1048</v>
       </c>
-      <c r="E36" s="55">
+      <c r="E36" s="41">
         <v>1605</v>
       </c>
-      <c r="F36" s="55">
+      <c r="F36" s="41">
         <v>15957</v>
       </c>
-      <c r="G36" s="56">
+      <c r="G36" s="42">
         <v>32273</v>
       </c>
     </row>
@@ -2160,8 +2159,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="D29:E29"/>
@@ -2178,6 +2175,8 @@
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>